<commit_message>
Update Review Log Sheet
</commit_message>
<xml_diff>
--- a/Review Log/Review Log Sheet.xlsx
+++ b/Review Log/Review Log Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Review No.</t>
   </si>
@@ -101,6 +101,36 @@
   <si>
     <t xml:space="preserve">Change the tasks time to meet
  the delivery deadline </t>
+  </si>
+  <si>
+    <t>RV_00_70</t>
+  </si>
+  <si>
+    <t>LM35 CDD</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>Kareem</t>
+  </si>
+  <si>
+    <t>RV_00_80</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Alhassan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to be organized </t>
+  </si>
+  <si>
+    <t>missing some requirements</t>
+  </si>
+  <si>
+    <t>RV_00_90</t>
   </si>
 </sst>
 </file>
@@ -459,17 +489,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -591,6 +621,57 @@
       </c>
       <c r="E7" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>